<commit_message>
Modified files according to first code review.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DariusDangi\Desktop\fwf-carturesti-internship-practice-performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E8CB6C-CDF7-4365-AEFE-FC4185AE5813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182D80B6-9D22-46AD-A9C5-4A8847294231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="585" windowWidth="27975" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="765" yWindow="585" windowWidth="27975" windowHeight="14055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>BestPickBooksQueue</t>
-  </si>
-  <si>
-    <t>BooksLimit</t>
   </si>
   <si>
     <t>InputMailAddresses</t>
@@ -695,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -779,170 +776,170 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
         <v>84</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>85</v>
-      </c>
-      <c r="C8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
         <v>49</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
         <v>52</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
         <v>55</v>
-      </c>
-      <c r="B12" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
         <v>57</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s">
         <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
         <v>62</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
         <v>64</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>65</v>
-      </c>
-      <c r="C19" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s">
         <v>67</v>
-      </c>
-      <c r="B20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>82</v>
-      </c>
-      <c r="C21" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" t="s">
         <v>88</v>
-      </c>
-      <c r="C25" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="C28" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -3089,8 +3086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3159,17 +3156,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>